<commit_message>
Updated project with multiple changes
</commit_message>
<xml_diff>
--- a/uploads/year 2.xlsx
+++ b/uploads/year 2.xlsx
@@ -945,7 +945,7 @@
   <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1259,9 +1259,6 @@
       <c r="H9">
         <v>50</v>
       </c>
-      <c r="I9">
-        <v>63</v>
-      </c>
       <c r="J9">
         <v>50</v>
       </c>

</xml_diff>